<commit_message>
Added the Extent Reports Functionality
</commit_message>
<xml_diff>
--- a/testData/SampleTestData.xlsx
+++ b/testData/SampleTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java_Selenium\OpenCart_HybridFramework\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B1B55F-67A3-49AA-B86B-860FCD4FFD57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B578D8-405D-45C4-8492-E14820757DFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{18A47E97-7256-4CE0-868B-FEDE9DA65846}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +506,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>